<commit_message>
Backup QR Scanner data - 4/6/2025, 4:53:45 PM
</commit_message>
<xml_diff>
--- a/backups/qr_scanner_backup_20250406_1653.xlsx
+++ b/backups/qr_scanner_backup_20250406_1653.xlsx
@@ -563,7 +563,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -704,9 +704,128 @@
         <v>13:31:22</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E9" t="str">
+        <v>16:53:19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E10" t="str">
+        <v>16:53:22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D11" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E11" t="str">
+        <v>16:53:25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D12" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E12" t="str">
+        <v>16:53:30</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D13" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E13" t="str">
+        <v>16:53:33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D14" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E14" t="str">
+        <v>16:53:36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>231249</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Jzbdhd</v>
+      </c>
+      <c r="D15" t="str">
+        <v>2025-04-06</v>
+      </c>
+      <c r="E15" t="str">
+        <v>16:53:40</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>